<commit_message>
counter verändert kein direkter reset
</commit_message>
<xml_diff>
--- a/unittests/7080gconnect/simcomconnect.xlsx
+++ b/unittests/7080gconnect/simcomconnect.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\github\pirmicboard_david\unittests\7080gconnect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952CAA52-0675-4D79-8FC2-0C1F4CDC4F4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9418D677-B6EA-4E44-98EE-10BBFE1CE9A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{216E3B78-6822-4185-B4FF-5583E01E67F4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{216E3B78-6822-4185-B4FF-5583E01E67F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>AT+CFUN=0</t>
   </si>
@@ -60,13 +61,64 @@
   </si>
   <si>
     <t>AT+CGATT=1</t>
+  </si>
+  <si>
+    <t>Board</t>
+  </si>
+  <si>
+    <t>Firmware</t>
+  </si>
+  <si>
+    <t>pirmicboard_david/unittests/7080gconnect/tmp_main_works_on_gpstracker.py at ccd93bc5e59aa4cae0e1f3a7a5dfe34171ab0504 · Qrist0ph/pirmicboard_david (github.com)</t>
+  </si>
+  <si>
+    <t>Sim CCID</t>
+  </si>
+  <si>
+    <t>2023-09-26 07:43:58 UTC</t>
+  </si>
+  <si>
+    <t>1nce</t>
+  </si>
+  <si>
+    <t>8988228066603839867</t>
+  </si>
+  <si>
+    <t>8988228066603839868</t>
+  </si>
+  <si>
+    <t>Start Bedingungen</t>
+  </si>
+  <si>
+    <t>Sim getauscht</t>
+  </si>
+  <si>
+    <t>2023-09-26 07:51:53 UTC</t>
+  </si>
+  <si>
+    <t>Counter</t>
+  </si>
+  <si>
+    <t>No Service, aber scheint dennoch online nach Runde 30</t>
+  </si>
+  <si>
+    <t>+CPSI: NO SERVICE,Online</t>
+  </si>
+  <si>
+    <t>+CPSI: LTE NB-IOT,Online,262-01,0xE2A4,35589386,84,EUTRAN-BAND8,3739,0,0,-10,-78,-67,11</t>
+  </si>
+  <si>
+    <t>10 Minutn laufen lassen</t>
+  </si>
+  <si>
+    <t>2023-09-26 08:06:55 UTC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,6 +131,19 @@
       <color rgb="FFCE9178"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF4A4A4A"/>
+      <name val="PortalFont"/>
     </font>
   </fonts>
   <fills count="2">
@@ -98,16 +163,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -422,13 +492,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3962215-3736-4F40-B74E-9096AE8F395A}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -436,7 +506,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -444,7 +514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -452,7 +522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -460,7 +530,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -468,15 +538,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -485,4 +555,111 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F8E28B8-7B50-45CB-9B1D-4C26BC0B0498}">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="41.6640625" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="46.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3">
+        <v>29</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="https://github.com/Qrist0ph/pirmicboard_david/blob/ccd93bc5e59aa4cae0e1f3a7a5dfe34171ab0504/unittests/7080gconnect/tmp_main_works_on_gpstracker.py" xr:uid="{ED57376D-E87D-4ED5-B400-0D17AA9BD25B}"/>
+    <hyperlink ref="C3" r:id="rId2" display="https://github.com/Qrist0ph/pirmicboard_david/blob/ccd93bc5e59aa4cae0e1f3a7a5dfe34171ab0504/unittests/7080gconnect/tmp_main_works_on_gpstracker.py" xr:uid="{149F73EE-C224-4D02-8450-32C7A3F534A6}"/>
+    <hyperlink ref="C4" r:id="rId3" display="https://github.com/Qrist0ph/pirmicboard_david/blob/ccd93bc5e59aa4cae0e1f3a7a5dfe34171ab0504/unittests/7080gconnect/tmp_main_works_on_gpstracker.py" xr:uid="{BF9EDEC2-4F2D-492A-98BF-8A4195669B0B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
tests in excel dokumentiert
</commit_message>
<xml_diff>
--- a/unittests/7080gconnect/simcomconnect.xlsx
+++ b/unittests/7080gconnect/simcomconnect.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\github\pirmicboard_david\unittests\7080gconnect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{748D1D4D-502B-4EC8-AB48-EE974F718FDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502DBB2E-8621-4C6D-A7DB-C3D0A7E29290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{216E3B78-6822-4185-B4FF-5583E01E67F4}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
   <si>
     <t>AT+CFUN=0</t>
   </si>
@@ -124,6 +124,24 @@
   </si>
   <si>
     <t>pirmicboard_david/unittests/7080gconnect/main.py at a2ef3bf7a16e352b20008353330c1dd8c7383065 · Qrist0ph/pirmicboard_david (github.com)</t>
+  </si>
+  <si>
+    <t>+COPS: 0,0,"Telekom.de 1nce.net",9</t>
+  </si>
+  <si>
+    <t>Geht online nach ca 40 runden</t>
+  </si>
+  <si>
+    <t>Online nach runde 27</t>
+  </si>
+  <si>
+    <t>Board getauscht</t>
+  </si>
+  <si>
+    <t>pirmicboard_david/unittests/7080gconnect/main.py at 5e8b1c0b49c3b408311a3a79990f6b82077685f9 · Qrist0ph/pirmicboard_david (github.com)</t>
+  </si>
+  <si>
+    <t>ein reset war notwendig, dann online gegangen</t>
   </si>
 </sst>
 </file>
@@ -571,10 +589,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F8E28B8-7B50-45CB-9B1D-4C26BC0B0498}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -686,14 +704,71 @@
         <v>26</v>
       </c>
     </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="https://github.com/Qrist0ph/pirmicboard_david/blob/ccd93bc5e59aa4cae0e1f3a7a5dfe34171ab0504/unittests/7080gconnect/tmp_main_works_on_gpstracker.py" xr:uid="{ED57376D-E87D-4ED5-B400-0D17AA9BD25B}"/>
     <hyperlink ref="C3" r:id="rId2" display="https://github.com/Qrist0ph/pirmicboard_david/blob/ccd93bc5e59aa4cae0e1f3a7a5dfe34171ab0504/unittests/7080gconnect/tmp_main_works_on_gpstracker.py" xr:uid="{149F73EE-C224-4D02-8450-32C7A3F534A6}"/>
     <hyperlink ref="C4" r:id="rId3" display="https://github.com/Qrist0ph/pirmicboard_david/blob/ccd93bc5e59aa4cae0e1f3a7a5dfe34171ab0504/unittests/7080gconnect/tmp_main_works_on_gpstracker.py" xr:uid="{BF9EDEC2-4F2D-492A-98BF-8A4195669B0B}"/>
     <hyperlink ref="C5" r:id="rId4" display="https://github.com/Qrist0ph/pirmicboard_david/blob/a2ef3bf7a16e352b20008353330c1dd8c7383065/unittests/7080gconnect/main.py" xr:uid="{6EF6CEF0-DBF4-42BC-BC01-DFEEB27AFB4C}"/>
+    <hyperlink ref="C6" r:id="rId5" display="https://github.com/Qrist0ph/pirmicboard_david/blob/a2ef3bf7a16e352b20008353330c1dd8c7383065/unittests/7080gconnect/main.py" xr:uid="{B789090C-FFA9-410A-B071-2C909142D6D4}"/>
+    <hyperlink ref="C7" r:id="rId6" display="https://github.com/Qrist0ph/pirmicboard_david/blob/5e8b1c0b49c3b408311a3a79990f6b82077685f9/unittests/7080gconnect/main.py" xr:uid="{22F56F1B-39FF-4D9B-B860-B71191CD7E99}"/>
+    <hyperlink ref="C8" r:id="rId7" display="https://github.com/Qrist0ph/pirmicboard_david/blob/5e8b1c0b49c3b408311a3a79990f6b82077685f9/unittests/7080gconnect/main.py" xr:uid="{17E7A5A7-9CCA-42FD-BB25-F112949E1A24}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
90 sek bug testcase
</commit_message>
<xml_diff>
--- a/unittests/7080gconnect/simcomconnect.xlsx
+++ b/unittests/7080gconnect/simcomconnect.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\github\pirmicboard_david\unittests\7080gconnect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502DBB2E-8621-4C6D-A7DB-C3D0A7E29290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D952CA-DC3B-4FBA-8993-96E6E01D7FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{216E3B78-6822-4185-B4FF-5583E01E67F4}"/>
+    <workbookView xWindow="3384" yWindow="3384" windowWidth="17280" windowHeight="9072" activeTab="2" xr2:uid="{216E3B78-6822-4185-B4FF-5583E01E67F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Modem Test" sheetId="2" r:id="rId2"/>
+    <sheet name="PIR Test" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
   <si>
     <t>AT+CFUN=0</t>
   </si>
@@ -142,6 +143,45 @@
   </si>
   <si>
     <t>ein reset war notwendig, dann online gegangen</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>PIR scheint sehr empfindlich</t>
+  </si>
+  <si>
+    <t>main.py</t>
+  </si>
+  <si>
+    <t>vebunden nach ca 30 run</t>
+  </si>
+  <si>
+    <t>Timestamp</t>
+  </si>
+  <si>
+    <t>PIR sieht gut aus</t>
+  </si>
+  <si>
+    <t>Fesnel</t>
+  </si>
+  <si>
+    <t>SR 501</t>
+  </si>
+  <si>
+    <t>90 Sek Bug</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Szenario</t>
+  </si>
+  <si>
+    <t>PIR unplugged</t>
+  </si>
+  <si>
+    <t>NEIN, wenn PIR unplugged</t>
   </si>
 </sst>
 </file>
@@ -197,7 +237,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -205,6 +245,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -589,186 +631,300 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F8E28B8-7B50-45CB-9B1D-4C26BC0B0498}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:J11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.6640625" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="46.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="79.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3">
+        <v>29</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="6">
+        <v>45196.387499999997</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="B10" s="5"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="B11" s="6"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="https://github.com/Qrist0ph/pirmicboard_david/blob/ccd93bc5e59aa4cae0e1f3a7a5dfe34171ab0504/unittests/7080gconnect/tmp_main_works_on_gpstracker.py" xr:uid="{ED57376D-E87D-4ED5-B400-0D17AA9BD25B}"/>
+    <hyperlink ref="D3" r:id="rId2" display="https://github.com/Qrist0ph/pirmicboard_david/blob/ccd93bc5e59aa4cae0e1f3a7a5dfe34171ab0504/unittests/7080gconnect/tmp_main_works_on_gpstracker.py" xr:uid="{149F73EE-C224-4D02-8450-32C7A3F534A6}"/>
+    <hyperlink ref="D4" r:id="rId3" display="https://github.com/Qrist0ph/pirmicboard_david/blob/ccd93bc5e59aa4cae0e1f3a7a5dfe34171ab0504/unittests/7080gconnect/tmp_main_works_on_gpstracker.py" xr:uid="{BF9EDEC2-4F2D-492A-98BF-8A4195669B0B}"/>
+    <hyperlink ref="D5" r:id="rId4" display="https://github.com/Qrist0ph/pirmicboard_david/blob/a2ef3bf7a16e352b20008353330c1dd8c7383065/unittests/7080gconnect/main.py" xr:uid="{6EF6CEF0-DBF4-42BC-BC01-DFEEB27AFB4C}"/>
+    <hyperlink ref="D6" r:id="rId5" display="https://github.com/Qrist0ph/pirmicboard_david/blob/a2ef3bf7a16e352b20008353330c1dd8c7383065/unittests/7080gconnect/main.py" xr:uid="{B789090C-FFA9-410A-B071-2C909142D6D4}"/>
+    <hyperlink ref="D7" r:id="rId6" display="https://github.com/Qrist0ph/pirmicboard_david/blob/5e8b1c0b49c3b408311a3a79990f6b82077685f9/unittests/7080gconnect/main.py" xr:uid="{22F56F1B-39FF-4D9B-B860-B71191CD7E99}"/>
+    <hyperlink ref="D8" r:id="rId7" display="https://github.com/Qrist0ph/pirmicboard_david/blob/5e8b1c0b49c3b408311a3a79990f6b82077685f9/unittests/7080gconnect/main.py" xr:uid="{17E7A5A7-9CCA-42FD-BB25-F112949E1A24}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43FF8DDF-3B80-40D7-8A15-8E52D62CFEF7}">
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="41.6640625" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="46.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="79.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" customWidth="1"/>
+    <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
       </c>
       <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="F1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+        <v>45</v>
+      </c>
+      <c r="G1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="6">
+        <v>45196.385416666664</v>
+      </c>
       <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>17</v>
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="6">
+        <v>45196.388888888891</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3">
-        <v>29</v>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" t="s">
+        <v>44</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
-        <v>23</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="6">
+        <v>45196.45</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" t="s">
-        <v>34</v>
+      <c r="E4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="https://github.com/Qrist0ph/pirmicboard_david/blob/ccd93bc5e59aa4cae0e1f3a7a5dfe34171ab0504/unittests/7080gconnect/tmp_main_works_on_gpstracker.py" xr:uid="{ED57376D-E87D-4ED5-B400-0D17AA9BD25B}"/>
-    <hyperlink ref="C3" r:id="rId2" display="https://github.com/Qrist0ph/pirmicboard_david/blob/ccd93bc5e59aa4cae0e1f3a7a5dfe34171ab0504/unittests/7080gconnect/tmp_main_works_on_gpstracker.py" xr:uid="{149F73EE-C224-4D02-8450-32C7A3F534A6}"/>
-    <hyperlink ref="C4" r:id="rId3" display="https://github.com/Qrist0ph/pirmicboard_david/blob/ccd93bc5e59aa4cae0e1f3a7a5dfe34171ab0504/unittests/7080gconnect/tmp_main_works_on_gpstracker.py" xr:uid="{BF9EDEC2-4F2D-492A-98BF-8A4195669B0B}"/>
-    <hyperlink ref="C5" r:id="rId4" display="https://github.com/Qrist0ph/pirmicboard_david/blob/a2ef3bf7a16e352b20008353330c1dd8c7383065/unittests/7080gconnect/main.py" xr:uid="{6EF6CEF0-DBF4-42BC-BC01-DFEEB27AFB4C}"/>
-    <hyperlink ref="C6" r:id="rId5" display="https://github.com/Qrist0ph/pirmicboard_david/blob/a2ef3bf7a16e352b20008353330c1dd8c7383065/unittests/7080gconnect/main.py" xr:uid="{B789090C-FFA9-410A-B071-2C909142D6D4}"/>
-    <hyperlink ref="C7" r:id="rId6" display="https://github.com/Qrist0ph/pirmicboard_david/blob/5e8b1c0b49c3b408311a3a79990f6b82077685f9/unittests/7080gconnect/main.py" xr:uid="{22F56F1B-39FF-4D9B-B860-B71191CD7E99}"/>
-    <hyperlink ref="C8" r:id="rId7" display="https://github.com/Qrist0ph/pirmicboard_david/blob/5e8b1c0b49c3b408311a3a79990f6b82077685f9/unittests/7080gconnect/main.py" xr:uid="{17E7A5A7-9CCA-42FD-BB25-F112949E1A24}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>